<commit_message>
Update Laporan Backlog, Burndown Chart, dan Log Book untuk Akhir Sprint 1
</commit_message>
<xml_diff>
--- a/BURNDOWN CHART.xlsx
+++ b/BURNDOWN CHART.xlsx
@@ -537,6 +537,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -545,30 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -599,6 +581,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -663,7 +663,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -765,7 +764,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -830,11 +828,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="123661896"/>
-        <c:axId val="123663072"/>
+        <c:axId val="128320528"/>
+        <c:axId val="128321312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="123661896"/>
+        <c:axId val="128320528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -876,7 +874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123663072"/>
+        <c:crossAx val="128321312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -884,7 +882,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123663072"/>
+        <c:axId val="128321312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +932,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123661896"/>
+        <c:crossAx val="128320528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1040,7 +1038,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1142,7 +1139,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1207,11 +1203,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="125165728"/>
-        <c:axId val="125166120"/>
+        <c:axId val="128322096"/>
+        <c:axId val="128322488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="125165728"/>
+        <c:axId val="128322096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,7 +1249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125166120"/>
+        <c:crossAx val="128322488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1261,7 +1257,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="125166120"/>
+        <c:axId val="128322488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1311,7 +1307,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125165728"/>
+        <c:crossAx val="128322096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1584,11 +1580,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="123148912"/>
-        <c:axId val="123148520"/>
+        <c:axId val="128323272"/>
+        <c:axId val="126128096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="123148912"/>
+        <c:axId val="128323272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1626,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123148520"/>
+        <c:crossAx val="126128096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1638,7 +1634,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123148520"/>
+        <c:axId val="126128096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1684,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="123148912"/>
+        <c:crossAx val="128323272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5113,13 +5109,13 @@
     </row>
     <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="11" t="s">
         <v>31</v>
       </c>
@@ -5131,13 +5127,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="12">
         <v>40</v>
       </c>
@@ -5145,28 +5141,28 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="37">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="31">
         <v>40</v>
       </c>
-      <c r="I14" s="39"/>
-      <c r="J14" s="29"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="29"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
@@ -5183,13 +5179,13 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="12">
         <v>40</v>
       </c>
@@ -5197,13 +5193,13 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="12">
         <v>40</v>
       </c>
@@ -5211,28 +5207,28 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="37">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="31">
         <v>60</v>
       </c>
-      <c r="I19" s="39"/>
-      <c r="J19" s="29"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="30"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="1" t="s">
@@ -5263,6 +5259,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:W7"/>
+    <mergeCell ref="C14:G15"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="C19:G20"/>
     <mergeCell ref="C12:G12"/>
@@ -5270,12 +5272,6 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="I19:I20"/>
-    <mergeCell ref="B2:W7"/>
-    <mergeCell ref="C14:G15"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="J14:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -5444,13 +5440,13 @@
     </row>
     <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="11" t="s">
         <v>31</v>
       </c>
@@ -5462,13 +5458,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="13">
         <v>40</v>
       </c>
@@ -5478,30 +5474,30 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="37">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="31">
         <v>40</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="33">
         <v>40</v>
       </c>
-      <c r="J14" s="29"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="29"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
@@ -5520,13 +5516,13 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="13">
         <v>40</v>
       </c>
@@ -5536,13 +5532,13 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="13">
         <v>40</v>
       </c>
@@ -5552,30 +5548,30 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="37">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="31">
         <v>60</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="33">
         <v>25</v>
       </c>
-      <c r="J19" s="29"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="30"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="1" t="s">
@@ -5606,12 +5602,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
     <mergeCell ref="B2:W7"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
@@ -5619,6 +5609,12 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5786,13 +5782,13 @@
     </row>
     <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="11" t="s">
         <v>31</v>
       </c>
@@ -5804,13 +5800,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="37"/>
       <c r="H13" s="18">
         <v>40</v>
       </c>
@@ -5822,32 +5818,32 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="37">
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="31">
         <v>40</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="33">
         <v>40</v>
       </c>
-      <c r="J14" s="29">
+      <c r="J14" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="29"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
@@ -5868,13 +5864,13 @@
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="40"/>
       <c r="H17" s="18">
         <v>40</v>
       </c>
@@ -5886,13 +5882,13 @@
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="37"/>
       <c r="H18" s="18">
         <v>40</v>
       </c>
@@ -5904,32 +5900,32 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="37">
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="31">
         <v>60</v>
       </c>
-      <c r="I19" s="39">
+      <c r="I19" s="33">
         <v>25</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="20">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="30"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="21"/>
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="1" t="s">
@@ -5960,6 +5956,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
     <mergeCell ref="B2:W7"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
@@ -5967,12 +5969,6 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Laporan hari ke 6 (Upadate Burndown Chart)
</commit_message>
<xml_diff>
--- a/BURNDOWN CHART.xlsx
+++ b/BURNDOWN CHART.xlsx
@@ -698,12 +698,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -712,6 +706,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -742,24 +760,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1022,11 +1022,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2051985424"/>
-        <c:axId val="-2051987056"/>
+        <c:axId val="1217284912"/>
+        <c:axId val="1217283280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2051985424"/>
+        <c:axId val="1217284912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,7 +1068,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051987056"/>
+        <c:crossAx val="1217283280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1076,7 +1076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2051987056"/>
+        <c:axId val="1217283280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,7 +1126,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051985424"/>
+        <c:crossAx val="1217284912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1397,11 +1397,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2051988144"/>
-        <c:axId val="-2051986512"/>
+        <c:axId val="1217280016"/>
+        <c:axId val="1217291440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2051988144"/>
+        <c:axId val="1217280016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,7 +1443,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051986512"/>
+        <c:crossAx val="1217291440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1451,7 +1451,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2051986512"/>
+        <c:axId val="1217291440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1501,7 +1501,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051988144"/>
+        <c:crossAx val="1217280016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1772,11 +1772,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-704290448"/>
-        <c:axId val="-704277936"/>
+        <c:axId val="1217277296"/>
+        <c:axId val="1217280560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-704290448"/>
+        <c:axId val="1217277296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1818,7 +1818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-704277936"/>
+        <c:crossAx val="1217280560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1826,7 +1826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-704277936"/>
+        <c:axId val="1217280560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1876,7 +1876,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-704290448"/>
+        <c:crossAx val="1217277296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2149,11 +2149,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2044553616"/>
-        <c:axId val="-2044551440"/>
+        <c:axId val="1217281648"/>
+        <c:axId val="1217281104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2044553616"/>
+        <c:axId val="1217281648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2195,7 +2195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044551440"/>
+        <c:crossAx val="1217281104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2203,7 +2203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2044551440"/>
+        <c:axId val="1217281104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2253,7 +2253,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044553616"/>
+        <c:crossAx val="1217281648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6251,13 +6251,13 @@
     </row>
     <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="11" t="s">
         <v>30</v>
       </c>
@@ -6269,13 +6269,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="12">
         <v>40</v>
       </c>
@@ -6283,28 +6283,28 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="46">
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="52">
         <v>40</v>
       </c>
-      <c r="I14" s="48"/>
-      <c r="J14" s="35"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="44"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="44"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
@@ -6321,13 +6321,13 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="3:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
       <c r="H17" s="12">
         <v>40</v>
       </c>
@@ -6335,13 +6335,13 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="12">
         <v>40</v>
       </c>
@@ -6349,28 +6349,28 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="46">
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="52">
         <v>60</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="35"/>
+      <c r="I19" s="54"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="36"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G21" s="1" t="s">
@@ -6401,12 +6401,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B2:W7"/>
-    <mergeCell ref="C14:G15"/>
-    <mergeCell ref="C13:G13"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="J14:J15"/>
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="C19:G20"/>
     <mergeCell ref="C12:G12"/>
@@ -6414,6 +6408,12 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="I19:I20"/>
+    <mergeCell ref="B2:W7"/>
+    <mergeCell ref="C14:G15"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="J14:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -6582,13 +6582,13 @@
     </row>
     <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="11" t="s">
         <v>30</v>
       </c>
@@ -6600,13 +6600,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="13">
         <v>40</v>
       </c>
@@ -6616,30 +6616,30 @@
       <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="46">
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="52">
         <v>40</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="54">
         <v>40</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="44"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="44"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
@@ -6658,13 +6658,13 @@
       <c r="J16" s="15"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
       <c r="H17" s="13">
         <v>40</v>
       </c>
@@ -6674,13 +6674,13 @@
       <c r="J17" s="15"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="13">
         <v>40</v>
       </c>
@@ -6690,30 +6690,30 @@
       <c r="J18" s="15"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="46">
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="52">
         <v>60</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="54">
         <v>25</v>
       </c>
-      <c r="J19" s="35"/>
+      <c r="J19" s="44"/>
     </row>
     <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="36"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G21" s="1" t="s">
@@ -6744,6 +6744,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
     <mergeCell ref="B2:W7"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
@@ -6751,12 +6757,6 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6926,13 +6926,13 @@
     </row>
     <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="45"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="51"/>
       <c r="H12" s="11" t="s">
         <v>30</v>
       </c>
@@ -6944,13 +6944,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="50" t="s">
+      <c r="C13" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="52"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="40"/>
       <c r="H13" s="18">
         <v>40</v>
       </c>
@@ -6962,32 +6962,32 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="46">
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="52">
         <v>40</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="54">
         <v>40</v>
       </c>
-      <c r="J14" s="35">
+      <c r="J14" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="44"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
@@ -7008,13 +7008,13 @@
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
       <c r="H17" s="18">
         <v>40</v>
       </c>
@@ -7026,13 +7026,13 @@
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="50" t="s">
+      <c r="C18" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
       <c r="H18" s="18">
         <v>40</v>
       </c>
@@ -7044,32 +7044,32 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="46">
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="52">
         <v>60</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="54">
         <v>25</v>
       </c>
-      <c r="J19" s="35">
+      <c r="J19" s="44">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="40"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="36"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G21" s="1" t="s">
@@ -7102,12 +7102,6 @@
     <row r="57" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
     <mergeCell ref="B2:W7"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
@@ -7115,6 +7109,12 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7125,8 +7125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7315,7 +7315,9 @@
       <c r="I13" s="27">
         <v>30</v>
       </c>
-      <c r="J13" s="28"/>
+      <c r="J13" s="28">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C14" s="68" t="s">
@@ -7325,13 +7327,15 @@
       <c r="E14" s="69"/>
       <c r="F14" s="69"/>
       <c r="G14" s="70"/>
-      <c r="H14" s="46">
+      <c r="H14" s="52">
         <v>45</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="54">
         <v>30</v>
       </c>
-      <c r="J14" s="35"/>
+      <c r="J14" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C15" s="68"/>
@@ -7339,9 +7343,9 @@
       <c r="E15" s="69"/>
       <c r="F15" s="69"/>
       <c r="G15" s="70"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="35"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="44"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C16" s="68"/>
@@ -7349,9 +7353,9 @@
       <c r="E16" s="69"/>
       <c r="F16" s="69"/>
       <c r="G16" s="70"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="44"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C17" s="65" t="s">
@@ -7367,7 +7371,9 @@
       <c r="I17" s="21">
         <v>60</v>
       </c>
-      <c r="J17" s="19"/>
+      <c r="J17" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C18" s="65" t="s">
@@ -7383,23 +7389,27 @@
       <c r="I18" s="21">
         <v>20</v>
       </c>
-      <c r="J18" s="19"/>
+      <c r="J18" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="50" t="s">
+      <c r="C19" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="52"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="40"/>
       <c r="H19" s="20">
         <v>40</v>
       </c>
       <c r="I19" s="21">
         <v>20</v>
       </c>
-      <c r="J19" s="19"/>
+      <c r="J19" s="19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C20" s="56" t="s">
@@ -7415,7 +7425,9 @@
       <c r="I20" s="29">
         <v>60</v>
       </c>
-      <c r="J20" s="30"/>
+      <c r="J20" s="30">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C21" s="23"/>

</xml_diff>

<commit_message>
Laporan Burndown Chart, Log Book Hari ke 8.
</commit_message>
<xml_diff>
--- a/BURNDOWN CHART.xlsx
+++ b/BURNDOWN CHART.xlsx
@@ -687,6 +687,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -696,6 +708,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -714,6 +744,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -722,36 +764,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -795,38 +807,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1058,11 +1058,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-219360272"/>
-        <c:axId val="-219363536"/>
+        <c:axId val="1372928560"/>
+        <c:axId val="1565347056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-219360272"/>
+        <c:axId val="1372928560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1104,7 +1104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-219363536"/>
+        <c:crossAx val="1565347056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1112,7 +1112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-219363536"/>
+        <c:axId val="1565347056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1162,7 +1162,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-219360272"/>
+        <c:crossAx val="1372928560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1435,11 +1435,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-219370608"/>
-        <c:axId val="-219359728"/>
+        <c:axId val="1565346512"/>
+        <c:axId val="1565349776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-219370608"/>
+        <c:axId val="1565346512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,7 +1481,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-219359728"/>
+        <c:crossAx val="1565349776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1489,7 +1489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-219359728"/>
+        <c:axId val="1565349776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,7 +1539,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-219370608"/>
+        <c:crossAx val="1565346512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1792,7 +1792,7 @@
                   <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1812,11 +1812,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-412880192"/>
-        <c:axId val="-412872032"/>
+        <c:axId val="1565343248"/>
+        <c:axId val="1565343792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-412880192"/>
+        <c:axId val="1565343248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1858,7 +1858,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-412872032"/>
+        <c:crossAx val="1565343792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1866,7 +1866,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-412872032"/>
+        <c:axId val="1565343792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1916,7 +1916,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-412880192"/>
+        <c:crossAx val="1565343248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3989,150 +3989,150 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
@@ -4202,155 +4202,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
@@ -4359,13 +4361,13 @@
     </row>
     <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="44"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58"/>
       <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
@@ -4377,13 +4379,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
-      <c r="G13" s="51"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="13">
         <v>40</v>
       </c>
@@ -4395,32 +4397,32 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="45">
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="47"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="52">
         <v>40</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="54">
         <v>40</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="36"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="34"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C16" s="4" t="s">
@@ -4441,13 +4443,13 @@
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="54"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="13">
         <v>40</v>
       </c>
@@ -4459,13 +4461,13 @@
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
       <c r="H18" s="13">
         <v>40</v>
       </c>
@@ -4477,32 +4479,32 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="45">
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="52">
         <v>60</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="54">
         <v>25</v>
       </c>
-      <c r="J19" s="34">
+      <c r="J19" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="39"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="35"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G21" s="1" t="s">
@@ -4535,12 +4537,6 @@
     <row r="57" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
     <mergeCell ref="B2:W7"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
@@ -4548,6 +4544,12 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4558,155 +4560,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
     </row>
     <row r="4" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
     </row>
     <row r="5" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
     </row>
     <row r="6" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
@@ -4715,13 +4719,13 @@
     </row>
     <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="19" t="s">
         <v>26</v>
       </c>
@@ -4733,13 +4737,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="63"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="26">
         <v>30</v>
       </c>
@@ -4751,51 +4755,51 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="45">
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="52">
         <v>45</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="54">
         <v>30</v>
       </c>
-      <c r="J14" s="34">
+      <c r="J14" s="38">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="34"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="34"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="64" t="s">
+      <c r="C17" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="65"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="66"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
       <c r="H17" s="15">
         <v>65</v>
       </c>
@@ -4807,13 +4811,13 @@
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="64" t="s">
+      <c r="C18" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="66"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="70"/>
       <c r="H18" s="15">
         <v>20</v>
       </c>
@@ -4825,13 +4829,13 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="45"/>
       <c r="H19" s="15">
         <v>40</v>
       </c>
@@ -4843,13 +4847,13 @@
       </c>
     </row>
     <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="55" t="s">
+      <c r="C20" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="57"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="61"/>
       <c r="H20" s="27">
         <v>65</v>
       </c>
@@ -4914,155 +4918,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
@@ -5071,13 +5077,13 @@
     </row>
     <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="19" t="s">
         <v>35</v>
       </c>
@@ -5089,93 +5095,103 @@
       </c>
     </row>
     <row r="13" spans="2:23" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="80" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="83"/>
-      <c r="H13" s="74">
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="34">
         <v>60</v>
       </c>
-      <c r="I13" s="22"/>
+      <c r="I13" s="22">
+        <v>35</v>
+      </c>
       <c r="J13" s="23"/>
     </row>
     <row r="14" spans="2:23" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="75">
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="83">
         <v>25</v>
       </c>
-      <c r="I14" s="47"/>
-      <c r="J14" s="34"/>
+      <c r="I14" s="54">
+        <v>25</v>
+      </c>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="2:23" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="75"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="34"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="2:23" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="34"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="83"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="38"/>
     </row>
     <row r="17" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="70" t="s">
+      <c r="C17" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="76">
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="35">
         <v>40</v>
       </c>
-      <c r="I17" s="30"/>
+      <c r="I17" s="30">
+        <v>25</v>
+      </c>
       <c r="J17" s="29"/>
     </row>
     <row r="18" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="68"/>
-      <c r="E18" s="68"/>
-      <c r="F18" s="68"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="76">
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="35">
         <v>50</v>
       </c>
-      <c r="I18" s="30"/>
+      <c r="I18" s="30">
+        <v>15</v>
+      </c>
       <c r="J18" s="29"/>
     </row>
     <row r="19" spans="3:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="79"/>
-      <c r="G19" s="80"/>
-      <c r="H19" s="77">
+      <c r="D19" s="78"/>
+      <c r="E19" s="78"/>
+      <c r="F19" s="78"/>
+      <c r="G19" s="79"/>
+      <c r="H19" s="36">
         <v>70</v>
       </c>
-      <c r="I19" s="24"/>
+      <c r="I19" s="24">
+        <v>40</v>
+      </c>
       <c r="J19" s="25"/>
     </row>
     <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5192,9 +5208,9 @@
       </c>
       <c r="I20" s="17">
         <f>SUM(I13:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="73">
+        <v>140</v>
+      </c>
+      <c r="J20" s="33">
         <f>SUM(J13:J19)</f>
         <v>0</v>
       </c>
@@ -5231,157 +5247,157 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5402,150 +5418,150 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="37"/>
+      <c r="W2" s="37"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
-      <c r="V3" s="33"/>
-      <c r="W3" s="33"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
-      <c r="V4" s="33"/>
-      <c r="W4" s="33"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="33"/>
-      <c r="V5" s="33"/>
-      <c r="W5" s="33"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="33"/>
-      <c r="T6" s="33"/>
-      <c r="U6" s="33"/>
-      <c r="V6" s="33"/>
-      <c r="W6" s="33"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="33"/>
-      <c r="T7" s="33"/>
-      <c r="U7" s="33"/>
-      <c r="V7" s="33"/>
-      <c r="W7" s="33"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Logbook dan burndown hari 10
</commit_message>
<xml_diff>
--- a/BURNDOWN CHART.xlsx
+++ b/BURNDOWN CHART.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Scrummaster" sheetId="20" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="53">
   <si>
     <t>Scrummaster</t>
   </si>
@@ -158,6 +158,27 @@
   <si>
     <t>Burndown Chart Sprint 4</t>
   </si>
+  <si>
+    <t>Penjelasan secara Umum : Aturan Permainan Dota2</t>
+  </si>
+  <si>
+    <t>Role : Support</t>
+  </si>
+  <si>
+    <t>Role : Durable</t>
+  </si>
+  <si>
+    <t>Role : Nuker</t>
+  </si>
+  <si>
+    <t>Warding : Jenis-Jenis Strategi Warding</t>
+  </si>
+  <si>
+    <t>Hero Guide Sniper : Best "Friends"</t>
+  </si>
+  <si>
+    <t>Jumat</t>
+  </si>
 </sst>
 </file>
 
@@ -203,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -595,11 +616,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -699,9 +757,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -710,60 +831,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -827,6 +894,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,6 +982,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -922,7 +1014,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="id-ID"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -979,7 +1071,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="id-ID"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -992,6 +1084,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1056,11 +1149,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1464790592"/>
-        <c:axId val="-1464786240"/>
+        <c:axId val="262430464"/>
+        <c:axId val="262431640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1464790592"/>
+        <c:axId val="262430464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,10 +1192,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1464786240"/>
+        <c:crossAx val="262431640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1110,7 +1203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1464786240"/>
+        <c:axId val="262431640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1157,10 +1250,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1464790592"/>
+        <c:crossAx val="262430464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1209,7 +1302,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="id-ID"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1298,7 +1391,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="id-ID"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1355,7 +1448,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="id-ID"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1433,11 +1526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1267274624"/>
-        <c:axId val="-1267278432"/>
+        <c:axId val="263173928"/>
+        <c:axId val="263174320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1267274624"/>
+        <c:axId val="263173928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1476,10 +1569,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1267278432"/>
+        <c:crossAx val="263174320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1487,7 +1580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1267278432"/>
+        <c:axId val="263174320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1534,10 +1627,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1267274624"/>
+        <c:crossAx val="263173928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1586,7 +1679,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="id-ID"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1675,7 +1768,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="id-ID"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1732,7 +1825,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="id-ID"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1810,11 +1903,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1267278976"/>
-        <c:axId val="-1267283872"/>
+        <c:axId val="263171184"/>
+        <c:axId val="263171576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1267278976"/>
+        <c:axId val="263171184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1853,10 +1946,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1267283872"/>
+        <c:crossAx val="263171576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1864,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1267283872"/>
+        <c:axId val="263171576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1911,10 +2004,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1267278976"/>
+        <c:crossAx val="263171184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1963,7 +2056,384 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="id-ID"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Burndown Chart </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="id-ID"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="id-ID"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 4'!$J$12:$L$12</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Rabu</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Kamis</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Jumat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$J$21:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>245</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="301104816"/>
+        <c:axId val="301098152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="301104816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="301098152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="301098152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="id-ID"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="301104816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="id-ID"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2094,6 +2564,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -3087,6 +3597,502 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3669,6 +4675,43 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>313765</xdr:colOff>
       <xdr:row>38</xdr:row>
+      <xdr:rowOff>77320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>1120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>77320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3984,155 +5027,155 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>4</v>
       </c>
@@ -4143,7 +5186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>1</v>
       </c>
@@ -4154,7 +5197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>2</v>
       </c>
@@ -4165,7 +5208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>3</v>
       </c>
@@ -4176,7 +5219,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>10</v>
       </c>
@@ -4200,172 +5243,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C12" s="38" t="s">
+    <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C12" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="61"/>
       <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
@@ -4376,14 +5419,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="41" t="s">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C13" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="43"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="48"/>
       <c r="H13" s="13">
         <v>40</v>
       </c>
@@ -4394,35 +5437,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="44" t="s">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C14" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47">
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="55">
         <v>40</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="57">
         <v>40</v>
       </c>
-      <c r="J14" s="49">
+      <c r="J14" s="41">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="44"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C15" s="49"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="41"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
         <v>21</v>
       </c>
@@ -4440,14 +5483,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="51" t="s">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="53"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="45"/>
       <c r="H17" s="13">
         <v>40</v>
       </c>
@@ -4458,14 +5501,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="41" t="s">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48"/>
       <c r="H18" s="13">
         <v>40</v>
       </c>
@@ -4476,35 +5519,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="44" t="s">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="47">
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="55">
         <v>60</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="57">
         <v>25</v>
       </c>
-      <c r="J19" s="49">
+      <c r="J19" s="41">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="54"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="56"/>
-      <c r="H20" s="57"/>
+    <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="52"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="56"/>
       <c r="I20" s="58"/>
-      <c r="J20" s="50"/>
-    </row>
-    <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J20" s="42"/>
+    </row>
+    <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="1" t="s">
         <v>22</v>
       </c>
@@ -4521,26 +5564,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="56" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="29.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
     <mergeCell ref="B2:W7"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
@@ -4548,6 +5585,12 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4559,171 +5602,171 @@
   <dimension ref="B2:W42"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+      <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-    </row>
-    <row r="3" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-    </row>
-    <row r="4" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-    </row>
-    <row r="5" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-    </row>
-    <row r="6" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-    </row>
-    <row r="7" spans="2:23" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+    </row>
+    <row r="5" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+    </row>
+    <row r="7" spans="2:23" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="62" t="s">
+    <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="19" t="s">
         <v>26</v>
       </c>
@@ -4734,14 +5777,14 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C13" s="65" t="s">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C13" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="26">
         <v>30</v>
       </c>
@@ -4752,52 +5795,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C14" s="71" t="s">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C14" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="47">
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="55">
         <v>45</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="57">
         <v>30</v>
       </c>
-      <c r="J14" s="49">
+      <c r="J14" s="41">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C15" s="71"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
-    </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C16" s="71"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="49"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C17" s="68" t="s">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C15" s="74"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="41"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="C16" s="74"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="55"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="41"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="72"/>
+      <c r="G17" s="73"/>
       <c r="H17" s="15">
         <v>65</v>
       </c>
@@ -4808,14 +5851,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C18" s="68" t="s">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="70"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="73"/>
       <c r="H18" s="15">
         <v>20</v>
       </c>
@@ -4826,14 +5869,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="41" t="s">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="48"/>
       <c r="H19" s="15">
         <v>40</v>
       </c>
@@ -4844,14 +5887,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C20" s="59" t="s">
+    <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="27">
         <v>65</v>
       </c>
@@ -4862,7 +5905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="18"/>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -4883,12 +5926,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
         <v>25</v>
       </c>
@@ -4916,172 +5959,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C12" s="62" t="s">
+    <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="67"/>
       <c r="H12" s="19" t="s">
         <v>35</v>
       </c>
@@ -5092,14 +6135,14 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:23" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="80" t="s">
+    <row r="13" spans="2:23" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="82"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="84"/>
+      <c r="F13" s="84"/>
+      <c r="G13" s="85"/>
       <c r="H13" s="34">
         <v>60</v>
       </c>
@@ -5110,52 +6153,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:23" ht="4.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="71" t="s">
+    <row r="14" spans="2:23" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="83">
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="86">
         <v>25</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="57">
         <v>25</v>
       </c>
-      <c r="J14" s="49">
+      <c r="J14" s="41">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:23" ht="6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="71"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="72"/>
-      <c r="G15" s="73"/>
-      <c r="H15" s="83"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
-    </row>
-    <row r="16" spans="2:23" ht="5.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="71"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="73"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="49"/>
-    </row>
-    <row r="17" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="74" t="s">
+    <row r="15" spans="2:23" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="74"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="41"/>
+    </row>
+    <row r="16" spans="2:23" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="74"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="41"/>
+    </row>
+    <row r="17" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="76"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="78"/>
+      <c r="F17" s="78"/>
+      <c r="G17" s="79"/>
       <c r="H17" s="35">
         <v>40</v>
       </c>
@@ -5166,14 +6209,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="71" t="s">
+    <row r="18" spans="3:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="72"/>
-      <c r="E18" s="72"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="73"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="76"/>
       <c r="H18" s="35">
         <v>50</v>
       </c>
@@ -5184,14 +6227,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C19" s="77" t="s">
+    <row r="19" spans="3:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="80" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="78"/>
-      <c r="E19" s="78"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="79"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="82"/>
       <c r="H19" s="36">
         <v>70</v>
       </c>
@@ -5202,7 +6245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -5223,12 +6266,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="1" t="s">
         <v>25</v>
       </c>
@@ -5253,165 +6296,335 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:W7"/>
+  <dimension ref="B2:W42"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E13" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="84"/>
+      <c r="G13" s="84"/>
+      <c r="H13" s="84"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="34">
+        <v>60</v>
+      </c>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E14" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="86">
+        <v>0</v>
+      </c>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E15" s="74"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="76"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="E16" s="74"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="93"/>
+      <c r="G17" s="93"/>
+      <c r="H17" s="93"/>
+      <c r="I17" s="94"/>
+      <c r="J17" s="39">
+        <v>40</v>
+      </c>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="93"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="39">
+        <v>40</v>
+      </c>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+    </row>
+    <row r="19" spans="5:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E19" s="90" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="91"/>
+      <c r="G19" s="91"/>
+      <c r="H19" s="91"/>
+      <c r="I19" s="92"/>
+      <c r="J19" s="39">
+        <v>55</v>
+      </c>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+    </row>
+    <row r="20" spans="5:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="87" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="36">
+        <v>50</v>
+      </c>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+    </row>
+    <row r="21" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="17">
+        <f>SUM(J13:J20)</f>
+        <v>245</v>
+      </c>
+      <c r="K21" s="17">
+        <f>SUM(K13:K20)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="33">
+        <f>SUM(L13:L20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="11">
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
     <mergeCell ref="B2:W7"/>
+    <mergeCell ref="E12:I12"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="L14:L16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5423,153 +6636,153 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-      <c r="R2" s="37"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="37"/>
-      <c r="U2" s="37"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-    </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="37"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="37"/>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="37"/>
-      <c r="P4" s="37"/>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="V4" s="37"/>
-      <c r="W4" s="37"/>
-    </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="37"/>
-      <c r="L5" s="37"/>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-      <c r="O5" s="37"/>
-      <c r="P5" s="37"/>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="37"/>
-      <c r="U5" s="37"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="37"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="40"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="40"/>
+      <c r="W5" s="40"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="40"/>
+      <c r="W7" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
logbook dan burndown chart hari 11
</commit_message>
<xml_diff>
--- a/BURNDOWN CHART.xlsx
+++ b/BURNDOWN CHART.xlsx
@@ -769,6 +769,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -784,24 +817,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -811,26 +826,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -895,6 +895,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -903,21 +918,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1149,11 +1149,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="262430464"/>
-        <c:axId val="262431640"/>
+        <c:axId val="258477528"/>
+        <c:axId val="258477920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="262430464"/>
+        <c:axId val="258477528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,7 +1195,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262431640"/>
+        <c:crossAx val="258477920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1203,7 +1203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262431640"/>
+        <c:axId val="258477920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1253,7 +1253,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262430464"/>
+        <c:crossAx val="258477528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1526,11 +1526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="263173928"/>
-        <c:axId val="263174320"/>
+        <c:axId val="258471256"/>
+        <c:axId val="258475176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="263173928"/>
+        <c:axId val="258471256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1572,7 +1572,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="263174320"/>
+        <c:crossAx val="258475176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1580,7 +1580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="263174320"/>
+        <c:axId val="258475176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1630,7 +1630,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="263173928"/>
+        <c:crossAx val="258471256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1903,11 +1903,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="263171184"/>
-        <c:axId val="263171576"/>
+        <c:axId val="258471648"/>
+        <c:axId val="258475568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="263171184"/>
+        <c:axId val="258471648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1949,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="263171576"/>
+        <c:crossAx val="258475568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1957,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="263171576"/>
+        <c:axId val="258475568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,7 +2007,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="263171184"/>
+        <c:crossAx val="258471648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2260,7 +2260,7 @@
                   <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2280,11 +2280,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="301104816"/>
-        <c:axId val="301098152"/>
+        <c:axId val="261144928"/>
+        <c:axId val="261150416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="301104816"/>
+        <c:axId val="261144928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2326,7 +2326,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301098152"/>
+        <c:crossAx val="261150416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2334,7 +2334,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="301098152"/>
+        <c:axId val="261150416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2384,7 +2384,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="301104816"/>
+        <c:crossAx val="261144928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5402,13 +5402,13 @@
     </row>
     <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C12" s="59" t="s">
+      <c r="C12" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43"/>
       <c r="H12" s="9" t="s">
         <v>17</v>
       </c>
@@ -5420,13 +5420,13 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="48"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="13">
         <v>40</v>
       </c>
@@ -5438,32 +5438,32 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="55">
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="50">
         <v>40</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I14" s="51">
         <v>40</v>
       </c>
-      <c r="J14" s="41">
+      <c r="J14" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="C15" s="49"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="41"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
@@ -5484,13 +5484,13 @@
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
       <c r="H17" s="13">
         <v>40</v>
       </c>
@@ -5502,13 +5502,13 @@
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="46"/>
       <c r="H18" s="13">
         <v>40</v>
       </c>
@@ -5520,32 +5520,32 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="49" t="s">
+      <c r="C19" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="55">
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="50">
         <v>60</v>
       </c>
-      <c r="I19" s="57">
+      <c r="I19" s="51">
         <v>25</v>
       </c>
-      <c r="J19" s="41">
+      <c r="J19" s="52">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="42"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="1" t="s">
@@ -5578,6 +5578,12 @@
     <row r="57" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="C19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
     <mergeCell ref="B2:W7"/>
     <mergeCell ref="C12:G12"/>
     <mergeCell ref="C13:G13"/>
@@ -5585,12 +5591,6 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="C19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5803,13 +5803,13 @@
       <c r="E14" s="75"/>
       <c r="F14" s="75"/>
       <c r="G14" s="76"/>
-      <c r="H14" s="55">
+      <c r="H14" s="50">
         <v>45</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I14" s="51">
         <v>30</v>
       </c>
-      <c r="J14" s="41">
+      <c r="J14" s="52">
         <v>0</v>
       </c>
     </row>
@@ -5819,9 +5819,9 @@
       <c r="E15" s="75"/>
       <c r="F15" s="75"/>
       <c r="G15" s="76"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="41"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
       <c r="C16" s="74"/>
@@ -5829,9 +5829,9 @@
       <c r="E16" s="75"/>
       <c r="F16" s="75"/>
       <c r="G16" s="76"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="41"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" s="71" t="s">
@@ -5870,13 +5870,13 @@
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="46" t="s">
+      <c r="C19" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="48"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="46"/>
       <c r="H19" s="15">
         <v>40</v>
       </c>
@@ -6164,10 +6164,10 @@
       <c r="H14" s="86">
         <v>25</v>
       </c>
-      <c r="I14" s="57">
+      <c r="I14" s="51">
         <v>25</v>
       </c>
-      <c r="J14" s="41">
+      <c r="J14" s="52">
         <v>0</v>
       </c>
     </row>
@@ -6178,8 +6178,8 @@
       <c r="F15" s="75"/>
       <c r="G15" s="76"/>
       <c r="H15" s="86"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="41"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
     </row>
     <row r="16" spans="2:23" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C16" s="74"/>
@@ -6188,8 +6188,8 @@
       <c r="F16" s="75"/>
       <c r="G16" s="76"/>
       <c r="H16" s="86"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="41"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
     </row>
     <row r="17" spans="3:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="77" t="s">
@@ -6298,8 +6298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6485,7 +6485,9 @@
       <c r="J13" s="34">
         <v>60</v>
       </c>
-      <c r="K13" s="34"/>
+      <c r="K13" s="34">
+        <v>30</v>
+      </c>
       <c r="L13" s="34"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
@@ -6499,10 +6501,12 @@
       <c r="J14" s="86">
         <v>0</v>
       </c>
-      <c r="K14" s="86"/>
+      <c r="K14" s="86">
+        <v>0</v>
+      </c>
       <c r="L14" s="86"/>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E15" s="74"/>
       <c r="F15" s="75"/>
       <c r="G15" s="75"/>
@@ -6512,7 +6516,7 @@
       <c r="K15" s="86"/>
       <c r="L15" s="86"/>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E16" s="74"/>
       <c r="F16" s="75"/>
       <c r="G16" s="75"/>
@@ -6526,56 +6530,64 @@
       <c r="E17" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="94"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="87"/>
+      <c r="I17" s="88"/>
       <c r="J17" s="39">
         <v>40</v>
       </c>
-      <c r="K17" s="39"/>
+      <c r="K17" s="39">
+        <v>0</v>
+      </c>
       <c r="L17" s="39"/>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="94"/>
+      <c r="F18" s="87"/>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="88"/>
       <c r="J18" s="39">
         <v>40</v>
       </c>
-      <c r="K18" s="39"/>
+      <c r="K18" s="39">
+        <v>40</v>
+      </c>
       <c r="L18" s="39"/>
     </row>
     <row r="19" spans="5:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="90" t="s">
+      <c r="E19" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="91"/>
-      <c r="G19" s="91"/>
-      <c r="H19" s="91"/>
-      <c r="I19" s="92"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="91"/>
       <c r="J19" s="39">
         <v>55</v>
       </c>
-      <c r="K19" s="39"/>
+      <c r="K19" s="39">
+        <v>20</v>
+      </c>
       <c r="L19" s="39"/>
     </row>
     <row r="20" spans="5:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="87" t="s">
+      <c r="E20" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="88"/>
-      <c r="G20" s="88"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="89"/>
+      <c r="F20" s="93"/>
+      <c r="G20" s="93"/>
+      <c r="H20" s="93"/>
+      <c r="I20" s="94"/>
       <c r="J20" s="36">
         <v>50</v>
       </c>
-      <c r="K20" s="36"/>
+      <c r="K20" s="36">
+        <v>15</v>
+      </c>
       <c r="L20" s="36"/>
     </row>
     <row r="21" spans="5:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6592,7 +6604,7 @@
       </c>
       <c r="K21" s="17">
         <f>SUM(K13:K20)</f>
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="L21" s="33">
         <f>SUM(L13:L20)</f>

</xml_diff>